<commit_message>
added parameterized test GitTestBurov_CreateIssuesFromFileTxtOrXlsx with System Property from using txt or xlsx file as parameters for test Also added xls source file and modified old files reader methods
</commit_message>
<xml_diff>
--- a/src/main/resources/data/excelParam.xlsx
+++ b/src/main/resources/data/excelParam.xlsx
@@ -26,27 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
-    <t>Test issue1</t>
-  </si>
-  <si>
-    <t>Test issue2</t>
-  </si>
-  <si>
-    <t>Test issue3</t>
-  </si>
-  <si>
-    <t>Test issue4</t>
-  </si>
-  <si>
-    <t>Test issue5</t>
-  </si>
-  <si>
-    <t>Test issue6</t>
-  </si>
-  <si>
-    <t>Test issue7</t>
-  </si>
-  <si>
     <t>Testing of addition a comment</t>
   </si>
   <si>
@@ -57,6 +36,27 @@
   </si>
   <si>
     <t>question</t>
+  </si>
+  <si>
+    <t>Test issueXLSX1</t>
+  </si>
+  <si>
+    <t>Test issueXLSX2</t>
+  </si>
+  <si>
+    <t>Test issueXLSX3</t>
+  </si>
+  <si>
+    <t>Test issueXLSX4</t>
+  </si>
+  <si>
+    <t>Test issueXLSX5</t>
+  </si>
+  <si>
+    <t>Test issueXLSX6</t>
+  </si>
+  <si>
+    <t>Test issueXLSX7</t>
   </si>
 </sst>
 </file>
@@ -377,12 +377,12 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -390,94 +390,94 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>